<commit_message>
term_dates table and csv. Unit times update.
Update to the unit times excel to prep for insert statement. Updated utilities with termdates insert and updated CSV to fit into table format.
</commit_message>
<xml_diff>
--- a/data/course_data/Units/Unit_Times.xlsx
+++ b/data/course_data/Units/Unit_Times.xlsx
@@ -1689,8 +1689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K378"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1826,7 +1826,7 @@
         <v>10</v>
       </c>
       <c r="H4" t="str">
-        <f t="shared" ref="H4:H67" si="0">IF(F4 = "9-13,15-20", "2,3,4,5,6,8,9,10,11,12,13", IF(F4 = "26-31,33-36,40-41", "14,15,16,17,18,19,21,22,23,24,25,26", ""))</f>
+        <f t="shared" ref="H4:H12" si="0">IF(F4 = "9-13,15-20", "2,3,4,5,6,8,9,10,11,12,13", IF(F4 = "26-31,33-36,40-41", "14,15,16,17,18,19,21,22,23,24,25,26", ""))</f>
         <v>2,3,4,5,6,8,9,10,11,12,13</v>
       </c>
       <c r="J4">
@@ -2156,7 +2156,7 @@
         <v>10</v>
       </c>
       <c r="H14" t="str">
-        <f t="shared" ref="H14:H77" si="1">IF(F14 = "9-13,15-20", "2,3,4,5,6,8,9,10,11,12,13", IF(F14 = "26-31,33-36,40-41", "14,15,16,17,18,19,21,22,23,24,25,26", IF(F14 = "26,28,30,33,35,40", "14,16,18,21,23,25", "")))</f>
+        <f t="shared" ref="H14" si="1">IF(F14 = "9-13,15-20", "2,3,4,5,6,8,9,10,11,12,13", IF(F14 = "26-31,33-36,40-41", "14,15,16,17,18,19,21,22,23,24,25,26", IF(F14 = "26,28,30,33,35,40", "14,16,18,21,23,25", "")))</f>
         <v>14,15,16,17,18,19,21,22,23,24,25,26</v>
       </c>
       <c r="J14">
@@ -2222,7 +2222,7 @@
         <v>10</v>
       </c>
       <c r="H16" t="str">
-        <f t="shared" ref="H16:H79" si="2">IF(F16 = "9-13,15-20", "2,3,4,5,6,8,9,10,11,12,13", IF(F16 = "26-31,33-36,40-41", "14,15,16,17,18,19,21,22,23,24,25,26", IF(F16 = "26,28,30,33,35,40", "14,16,18,21,23,25", IF(F16 = "9,11,13,16,18,20", "2,4,6,9,11,13", ""))))</f>
+        <f t="shared" ref="H16" si="2">IF(F16 = "9-13,15-20", "2,3,4,5,6,8,9,10,11,12,13", IF(F16 = "26-31,33-36,40-41", "14,15,16,17,18,19,21,22,23,24,25,26", IF(F16 = "26,28,30,33,35,40", "14,16,18,21,23,25", IF(F16 = "9,11,13,16,18,20", "2,4,6,9,11,13", ""))))</f>
         <v>2,3,4,5,6,8,9,10,11,12,13</v>
       </c>
       <c r="J16">
@@ -2319,7 +2319,7 @@
         <v>19</v>
       </c>
       <c r="H19" t="str">
-        <f t="shared" ref="H18:H81" si="3">IF(F19 = "9-13,15-20", "2,3,4,5,6,8,9,10,11,12,13", IF(F19 = "26-31,33-36,40-41", "14,15,16,17,18,19,21,22,23,24,25,26", IF(F19 = "26,28,30,33,35,40", "14,16,18,21,23,25", IF(F19 = "9,11,13,16,18,20", "2,4,6,9,11,13", IF(F19 = 19, "12", "")))))</f>
+        <f t="shared" ref="H19:H20" si="3">IF(F19 = "9-13,15-20", "2,3,4,5,6,8,9,10,11,12,13", IF(F19 = "26-31,33-36,40-41", "14,15,16,17,18,19,21,22,23,24,25,26", IF(F19 = "26,28,30,33,35,40", "14,16,18,21,23,25", IF(F19 = "9,11,13,16,18,20", "2,4,6,9,11,13", IF(F19 = 19, "12", "")))))</f>
         <v>14,16,18,21,23,25</v>
       </c>
       <c r="J19">
@@ -2482,7 +2482,7 @@
         <v>44</v>
       </c>
       <c r="H24" t="str">
-        <f t="shared" ref="H24:H87" si="4">IF(F24 = "9-13,15-20", "2,3,4,5,6,8,9,10,11,12,13", IF(F24 = "26-31,33-36,40-41", "14,15,16,17,18,19,21,22,23,24,25,26", IF(F24 = "26,28,30,33,35,40", "14,16,18,21,23,25", IF(F24 = "9,11,13,16,18,20", "2,4,6,9,11,13", IF(F24 = "9,11,13,15,17,19", "2,4,6,8,10,12", "")))))</f>
+        <f t="shared" ref="H24" si="4">IF(F24 = "9-13,15-20", "2,3,4,5,6,8,9,10,11,12,13", IF(F24 = "26-31,33-36,40-41", "14,15,16,17,18,19,21,22,23,24,25,26", IF(F24 = "26,28,30,33,35,40", "14,16,18,21,23,25", IF(F24 = "9,11,13,16,18,20", "2,4,6,9,11,13", IF(F24 = "9,11,13,15,17,19", "2,4,6,8,10,12", "")))))</f>
         <v>2,4,6,8,10,12</v>
       </c>
       <c r="J24">
@@ -2542,7 +2542,7 @@
         <v>44</v>
       </c>
       <c r="H26" t="str">
-        <f t="shared" ref="H26:H89" si="5">IF(F26 = "9-13,15-20", "2,3,4,5,6,8,9,10,11,12,13", IF(F26 = "26-31,33-36,40-41", "14,15,16,17,18,19,21,22,23,24,25,26", IF(F26 = "26,28,30,33,35,40", "14,16,18,21,23,25", IF(F26 = "9,11,13,16,18,20", "2,4,6,9,11,13", IF(F26 = "9,11,13,15,17,19", "2,4,6,8,10,12", IF(F26 = "27,29,31,33,35,40", "15,17,19,21,23,25", ""))))))</f>
+        <f t="shared" ref="H26" si="5">IF(F26 = "9-13,15-20", "2,3,4,5,6,8,9,10,11,12,13", IF(F26 = "26-31,33-36,40-41", "14,15,16,17,18,19,21,22,23,24,25,26", IF(F26 = "26,28,30,33,35,40", "14,16,18,21,23,25", IF(F26 = "9,11,13,16,18,20", "2,4,6,9,11,13", IF(F26 = "9,11,13,15,17,19", "2,4,6,8,10,12", IF(F26 = "27,29,31,33,35,40", "15,17,19,21,23,25", ""))))))</f>
         <v>15,17,19,21,23,25</v>
       </c>
     </row>
@@ -2674,7 +2674,7 @@
         <v>25</v>
       </c>
       <c r="H31" t="str">
-        <f t="shared" ref="H28:H91" si="6">IF(F31 = "9-13,15-20", "2,3,4,5,6,8,9,10,11,12,13", IF(F31 = "26-31,33-36,40-41", "14,15,16,17,18,19,21,22,23,24,25,26", IF(F31 = "26,28,30,33,35,40", "14,16,18,21,23,25", IF(F31 = "9,11,13,16,18,20", "2,4,6,9,11,13", IF(F31 = "9,11,13,15,17,19", "2,4,6,8,10,12", IF(F31 = "27,29,31,33,35,40", "15,17,19,21,23,25", IF(F31 = "9,13,16,18,20", "2,6,9,11,13", "")))))))</f>
+        <f t="shared" ref="H31:H90" si="6">IF(F31 = "9-13,15-20", "2,3,4,5,6,8,9,10,11,12,13", IF(F31 = "26-31,33-36,40-41", "14,15,16,17,18,19,21,22,23,24,25,26", IF(F31 = "26,28,30,33,35,40", "14,16,18,21,23,25", IF(F31 = "9,11,13,16,18,20", "2,4,6,9,11,13", IF(F31 = "9,11,13,15,17,19", "2,4,6,8,10,12", IF(F31 = "27,29,31,33,35,40", "15,17,19,21,23,25", IF(F31 = "9,13,16,18,20", "2,6,9,11,13", "")))))))</f>
         <v>14,15,16,17,18,19,21,22,23,24,25,26</v>
       </c>
     </row>
@@ -4498,7 +4498,7 @@
         <v>10</v>
       </c>
       <c r="H100" t="str">
-        <f t="shared" ref="H92:H155" si="7">IF(F100 = "9-13,15-20", "2,3,4,5,6,8,9,10,11,12,13", IF(F100 = "26-31,33-36,40-41", "14,15,16,17,18,19,21,22,23,24,25,26", IF(F100 = "26,28,30,33,35,40", "14,16,18,21,23,25", IF(F100 = "9,11,13,16,18,20", "2,4,6,9,11,13", IF(F100 = "9,11,13,15,17,19", "2,4,6,8,10,12", IF(F100 = "27,29,31,33,35,40", "15,17,19,21,23,25", IF(F100 = "9,13,16,18,20", "2,6,9,11,13", "")))))))</f>
+        <f t="shared" ref="H100:H145" si="7">IF(F100 = "9-13,15-20", "2,3,4,5,6,8,9,10,11,12,13", IF(F100 = "26-31,33-36,40-41", "14,15,16,17,18,19,21,22,23,24,25,26", IF(F100 = "26,28,30,33,35,40", "14,16,18,21,23,25", IF(F100 = "9,11,13,16,18,20", "2,4,6,9,11,13", IF(F100 = "9,11,13,15,17,19", "2,4,6,8,10,12", IF(F100 = "27,29,31,33,35,40", "15,17,19,21,23,25", IF(F100 = "9,13,16,18,20", "2,6,9,11,13", "")))))))</f>
         <v>2,3,4,5,6,8,9,10,11,12,13</v>
       </c>
     </row>
@@ -5971,7 +5971,7 @@
         <v>25</v>
       </c>
       <c r="H156" t="str">
-        <f t="shared" ref="H156:H219" si="8">IF(F156 = "9-13,15-20", "2,3,4,5,6,8,9,10,11,12,13", IF(F156 = "26-31,33-36,40-41", "14,15,16,17,18,19,21,22,23,24,25,26", IF(F156 = "26,28,30,33,35,40", "14,16,18,21,23,25", IF(F156 = "9,11,13,16,18,20", "2,4,6,9,11,13", IF(F156 = "9,11,13,15,17,19", "2,4,6,8,10,12", IF(F156 = "27,29,31,33,35,40", "15,17,19,21,23,25", IF(F156 = "9,13,16,18,20", "2,6,9,11,13", "")))))))</f>
+        <f t="shared" ref="H156:H216" si="8">IF(F156 = "9-13,15-20", "2,3,4,5,6,8,9,10,11,12,13", IF(F156 = "26-31,33-36,40-41", "14,15,16,17,18,19,21,22,23,24,25,26", IF(F156 = "26,28,30,33,35,40", "14,16,18,21,23,25", IF(F156 = "9,11,13,16,18,20", "2,4,6,9,11,13", IF(F156 = "9,11,13,15,17,19", "2,4,6,8,10,12", IF(F156 = "27,29,31,33,35,40", "15,17,19,21,23,25", IF(F156 = "9,13,16,18,20", "2,6,9,11,13", "")))))))</f>
         <v>2,3,4,5,6,8,9,10,11,12,13</v>
       </c>
     </row>
@@ -7887,7 +7887,7 @@
         <v>127</v>
       </c>
       <c r="H229" t="str">
-        <f t="shared" ref="H220:H283" si="9">IF(F229 = "9-13,15-20", "2,3,4,5,6,8,9,10,11,12,13", IF(F229 = "26-31,33-36,40-41", "14,15,16,17,18,19,21,22,23,24,25,26", IF(F229 = "26,28,30,33,35,40", "14,16,18,21,23,25", IF(F229 = "9,11,13,16,18,20", "2,4,6,9,11,13", IF(F229 = "9,11,13,15,17,19", "2,4,6,8,10,12", IF(F229 = "27,29,31,33,35,40", "15,17,19,21,23,25", IF(F229 = "9,13,16,18,20", "2,6,9,11,13", "")))))))</f>
+        <f t="shared" ref="H229:H259" si="9">IF(F229 = "9-13,15-20", "2,3,4,5,6,8,9,10,11,12,13", IF(F229 = "26-31,33-36,40-41", "14,15,16,17,18,19,21,22,23,24,25,26", IF(F229 = "26,28,30,33,35,40", "14,16,18,21,23,25", IF(F229 = "9,11,13,16,18,20", "2,4,6,9,11,13", IF(F229 = "9,11,13,15,17,19", "2,4,6,8,10,12", IF(F229 = "27,29,31,33,35,40", "15,17,19,21,23,25", IF(F229 = "9,13,16,18,20", "2,6,9,11,13", "")))))))</f>
         <v>2,3,4,5,6,8,9,10,11,12,13</v>
       </c>
     </row>
@@ -9355,7 +9355,7 @@
         <v>10</v>
       </c>
       <c r="H285" t="str">
-        <f t="shared" ref="H284:H347" si="10">IF(F285 = "9-13,15-20", "2,3,4,5,6,8,9,10,11,12,13", IF(F285 = "26-31,33-36,40-41", "14,15,16,17,18,19,21,22,23,24,25,26", IF(F285 = "26,28,30,33,35,40", "14,16,18,21,23,25", IF(F285 = "9,11,13,16,18,20", "2,4,6,9,11,13", IF(F285 = "9,11,13,15,17,19", "2,4,6,8,10,12", IF(F285 = "27,29,31,33,35,40", "15,17,19,21,23,25", IF(F285 = "9,13,16,18,20", "2,6,9,11,13", "")))))))</f>
+        <f t="shared" ref="H285:H345" si="10">IF(F285 = "9-13,15-20", "2,3,4,5,6,8,9,10,11,12,13", IF(F285 = "26-31,33-36,40-41", "14,15,16,17,18,19,21,22,23,24,25,26", IF(F285 = "26,28,30,33,35,40", "14,16,18,21,23,25", IF(F285 = "9,11,13,16,18,20", "2,4,6,9,11,13", IF(F285 = "9,11,13,15,17,19", "2,4,6,8,10,12", IF(F285 = "27,29,31,33,35,40", "15,17,19,21,23,25", IF(F285 = "9,13,16,18,20", "2,6,9,11,13", "")))))))</f>
         <v>2,3,4,5,6,8,9,10,11,12,13</v>
       </c>
     </row>

</xml_diff>